<commit_message>
Clean up of code and repo (anything with X_ is extra code that is not necessary for the publication, psa, or figures)
</commit_message>
<xml_diff>
--- a/analysis/data/raw/vac_cov.xlsx
+++ b/analysis/data/raw/vac_cov.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/halliebenjamin/Documents/GitHub/roiv/analysis/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80806083-D73F-9240-BA3C-E5AC70B59C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA6DF60-32C8-744C-88BC-764DDB676258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{400003AA-9577-F740-A0D3-407B36423847}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" xr2:uid="{400003AA-9577-F740-A0D3-407B36423847}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>EGY</t>
   </si>
   <si>
-    <t>EIR</t>
-  </si>
-  <si>
     <t>ESP</t>
   </si>
   <si>
@@ -293,9 +290,6 @@
     <t>JOR</t>
   </si>
   <si>
-    <t>JAP</t>
-  </si>
-  <si>
     <t>KAZ</t>
   </si>
   <si>
@@ -576,6 +570,12 @@
   </si>
   <si>
     <t>ZWE</t>
+  </si>
+  <si>
+    <t>JPN</t>
+  </si>
+  <si>
+    <t>ERI</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -630,8 +630,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6601353F-8031-E147-8CCD-B8FF9919A049}">
   <dimension ref="A1:B179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="116" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>179</v>
       </c>
       <c r="B51" s="3">
         <v>0</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3">
         <v>0.80600000000000005</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3">
         <v>0.60099999999999998</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3">
         <v>1.23E-2</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3">
         <v>0.73399999999999999</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3">
         <v>0.65600000000000003</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3">
         <v>0.70799999999999996</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="3">
         <v>6.8400000000000002E-2</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="3">
         <v>0.68400000000000005</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="3">
         <v>0.26</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="3">
         <v>4.1700000000000001E-2</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="3">
         <v>6.0400000000000002E-2</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3">
         <v>9.1499999999999998E-2</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="3">
         <v>1.0200000000000001E-2</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3">
         <v>0.13700000000000001</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3">
         <v>0.64700000000000002</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" s="3">
         <v>0.308</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3">
         <v>0.23400000000000001</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3">
         <v>0.35899999999999999</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3">
         <v>0.60399999999999998</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3">
         <v>0.38800000000000001</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3">
         <v>0.47299999999999998</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3">
         <v>6.0099999999999997E-3</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3">
         <v>0.61</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75" s="3">
         <v>0.36399999999999999</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="3">
         <v>0.35299999999999998</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="3">
         <v>0.76800000000000002</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3">
         <v>0.57099999999999995</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="3">
         <v>0.122</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="3">
         <v>0.76500000000000001</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" s="3">
         <v>0.624</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" s="3">
         <v>0.73299999999999998</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" s="3">
         <v>0.17799999999999999</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" s="3">
         <v>0.37</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="B85" s="3">
         <v>0.77700000000000002</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B86" s="3">
         <v>0.433</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B87" s="3">
         <v>5.67E-2</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88" s="3">
         <v>0.14000000000000001</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B89" s="3">
         <v>0.79800000000000004</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" s="3">
         <v>0.81100000000000005</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B91" s="3">
         <v>0.73399999999999999</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B92" s="3">
         <v>0.44700000000000001</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B93" s="3">
         <v>0.255</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B94" s="3">
         <v>0.111</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B95" s="3">
         <v>0.104</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B96" s="3">
         <v>0.25700000000000001</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B97" s="3">
         <v>0.64100000000000001</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B98" s="3">
         <v>0.28599999999999998</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B99" s="3">
         <v>0.66900000000000004</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B100" s="3">
         <v>0.67700000000000005</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B101" s="3">
         <v>0.65400000000000003</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102" s="3">
         <v>0.61199999999999999</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B103" s="3">
         <v>0.23599999999999999</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B104" s="3">
         <v>1.95E-2</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B105" s="3">
         <v>0.67200000000000004</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B106" s="3">
         <v>0.503</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B107" s="3">
         <v>0.38500000000000001</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B108" s="3">
         <v>1.6E-2</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B109" s="3">
         <v>0.84</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B110" s="3">
         <v>0.23200000000000001</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B111" s="3">
         <v>0.41599999999999998</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B112" s="3">
         <v>0.64700000000000002</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B113" s="3">
         <v>0.13300000000000001</v>
@@ -1883,7 +1883,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B114" s="3">
         <v>0.14599999999999999</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B115" s="3">
         <v>0.70299999999999996</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B116" s="3">
         <v>3.1699999999999999E-2</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B117" s="3">
         <v>0.77900000000000003</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B118" s="3">
         <v>0.12</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B119" s="3">
         <v>2.35E-2</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B120" s="3">
         <v>1.8200000000000001E-2</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B121" s="3">
         <v>0.373</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B122" s="3">
         <v>0.70599999999999996</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B123" s="3">
         <v>0.70899999999999996</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B124" s="3">
         <v>0.29899999999999999</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B125" s="3">
         <v>0.72599999999999998</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B126" s="3">
         <v>0.54700000000000004</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B127" s="3">
         <v>0.24199999999999999</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B128" s="3">
         <v>0.55700000000000005</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B129" s="3">
         <v>0.58699999999999997</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B130" s="3">
         <v>0.35599999999999998</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B131" s="3">
         <v>2.29E-2</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B132" s="3">
         <v>0.54500000000000004</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B133" s="3">
         <v>0.88700000000000001</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B134" s="3">
         <v>0.38100000000000001</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B135" s="3">
         <v>0.27100000000000002</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B136" s="3">
         <v>0.75700000000000001</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B137" s="3">
         <v>0.36599999999999999</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B138" s="3">
         <v>0.40799999999999997</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B139" s="3">
         <v>0.316</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B140" s="3">
         <v>0.64300000000000002</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B141" s="3">
         <v>2.75E-2</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B142" s="3">
         <v>5.4300000000000001E-2</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B143" s="3">
         <v>0.85299999999999998</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B144" s="3">
         <v>4.5199999999999997E-2</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B145" s="3">
         <v>0.629</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B146" s="3">
         <v>4.0399999999999998E-2</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B147" s="3">
         <v>0.45900000000000002</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B148" s="3">
         <v>1.5299999999999999E-2</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B149" s="3">
         <v>0.216</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B150" s="3">
         <v>0.377</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B151" s="3">
         <v>0.47399999999999998</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B152" s="3">
         <v>0.55900000000000005</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B153" s="3">
         <v>0.70899999999999996</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B154" s="3">
         <v>0.24099999999999999</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B155" s="3">
         <v>0.79</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B156" s="3">
         <v>4.1399999999999999E-2</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B157" s="3">
         <v>4.6299999999999996E-3</v>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B158" s="3">
         <v>9.01E-2</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B159" s="3">
         <v>0.61699999999999999</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B160" s="3">
         <v>0.27</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B161" s="3">
         <v>0.36699999999999999</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B162" s="3">
         <v>0.46400000000000002</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B163" s="3">
         <v>0.443</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B164" s="3">
         <v>0.59699999999999998</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B165" s="3">
         <v>0.61699999999999999</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B166" s="3">
         <v>1.7899999999999999E-2</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B167" s="3">
         <v>2.7E-2</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B168" s="3">
         <v>0.28000000000000003</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B169" s="3">
         <v>0.76500000000000001</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B170" s="3">
         <v>0.61</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B171" s="3">
         <v>0.316</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B172" s="3">
         <v>0.216</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B173" s="3">
         <v>0.374</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B174" s="3">
         <v>0.56999999999999995</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B175" s="3">
         <v>0.14599999999999999</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B176" s="3">
         <v>8.3999999999999995E-3</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B177" s="3">
         <v>0.253</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B178" s="3">
         <v>4.1700000000000001E-2</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B179" s="3">
         <v>0.19400000000000001</v>

</xml_diff>